<commit_message>
SDGS-61 edited make_sdgbubbleplot in postprocess
</commit_message>
<xml_diff>
--- a/keywords/keywords_expanded_manually_reordered.xlsx
+++ b/keywords/keywords_expanded_manually_reordered.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FDFEB2-37FF-4C1A-8B62-7E0406324B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BB9B68-DC80-4D65-98D3-7B3B82D188E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9556,11 +9556,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9902,10 +9906,13 @@
   <dimension ref="A1:BH187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9914,7 +9921,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1">
@@ -10096,7 +10103,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
@@ -10146,7 +10153,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
@@ -10190,7 +10197,7 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
@@ -10237,7 +10244,7 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
@@ -10323,7 +10330,7 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
@@ -10391,7 +10398,7 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
@@ -10480,7 +10487,7 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
@@ -10509,7 +10516,7 @@
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
@@ -10544,7 +10551,7 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>124</v>
       </c>
       <c r="D10" t="s">
@@ -10567,7 +10574,7 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>125</v>
       </c>
       <c r="D11" t="s">
@@ -10668,7 +10675,7 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>126</v>
       </c>
       <c r="D12" t="s">
@@ -10730,7 +10737,7 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>127</v>
       </c>
       <c r="D13" t="s">
@@ -10786,7 +10793,7 @@
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D14" t="s">
@@ -10851,7 +10858,7 @@
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D15" t="s">
@@ -10910,7 +10917,7 @@
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D16" t="s">
@@ -10948,7 +10955,7 @@
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>131</v>
       </c>
       <c r="D17" t="s">
@@ -10977,7 +10984,7 @@
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D18" t="s">
@@ -11021,7 +11028,7 @@
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D19" t="s">
@@ -11092,7 +11099,7 @@
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D20" t="s">
@@ -11145,7 +11152,7 @@
       <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D21" t="s">
@@ -11186,7 +11193,7 @@
       <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>136</v>
       </c>
       <c r="D22" t="s">
@@ -11239,7 +11246,7 @@
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D23" t="s">
@@ -11295,7 +11302,7 @@
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>138</v>
       </c>
       <c r="D24" t="s">
@@ -11351,7 +11358,7 @@
       <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>139</v>
       </c>
       <c r="D25" t="s">
@@ -11404,7 +11411,7 @@
       <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D26" t="s">
@@ -11463,7 +11470,7 @@
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D27" t="s">
@@ -11540,7 +11547,7 @@
       <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D28" t="s">
@@ -11722,7 +11729,7 @@
       <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D29" t="s">
@@ -11751,7 +11758,7 @@
       <c r="B30" t="s">
         <v>12</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D30" t="s">
@@ -11816,7 +11823,7 @@
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>145</v>
       </c>
       <c r="D31" t="s">
@@ -11833,7 +11840,7 @@
       <c r="B32" t="s">
         <v>12</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D32" t="s">
@@ -11931,7 +11938,7 @@
       <c r="B33" t="s">
         <v>13</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D33" t="s">
@@ -11999,7 +12006,7 @@
       <c r="B34" t="s">
         <v>13</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>148</v>
       </c>
       <c r="D34" t="s">
@@ -12061,7 +12068,7 @@
       <c r="B35" t="s">
         <v>13</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D35" t="s">
@@ -12129,7 +12136,7 @@
       <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>150</v>
       </c>
       <c r="D36" t="s">
@@ -12176,7 +12183,7 @@
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D37" t="s">
@@ -12235,7 +12242,7 @@
       <c r="B38" t="s">
         <v>13</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>152</v>
       </c>
       <c r="D38" t="s">
@@ -12318,7 +12325,7 @@
       <c r="B39" t="s">
         <v>13</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D39" t="s">
@@ -12380,7 +12387,7 @@
       <c r="B40" t="s">
         <v>13</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D40" t="s">
@@ -12508,7 +12515,7 @@
       <c r="B41" t="s">
         <v>13</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D41" t="s">
@@ -12615,7 +12622,7 @@
       <c r="B42" t="s">
         <v>13</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D42" t="s">
@@ -12683,7 +12690,7 @@
       <c r="B43" t="s">
         <v>13</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>157</v>
       </c>
       <c r="D43" t="s">
@@ -12730,7 +12737,7 @@
       <c r="B44" t="s">
         <v>14</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D44" t="s">
@@ -12903,7 +12910,7 @@
       <c r="B45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="3" t="s">
         <v>159</v>
       </c>
       <c r="D45" t="s">
@@ -12983,7 +12990,7 @@
       <c r="B46" t="s">
         <v>14</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>160</v>
       </c>
       <c r="D46" t="s">
@@ -13069,7 +13076,7 @@
       <c r="B47" t="s">
         <v>14</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="3" t="s">
         <v>161</v>
       </c>
       <c r="D47" t="s">
@@ -13104,7 +13111,7 @@
       <c r="B48" t="s">
         <v>14</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
         <v>162</v>
       </c>
       <c r="D48" t="s">
@@ -13139,7 +13146,7 @@
       <c r="B49" t="s">
         <v>14</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
         <v>163</v>
       </c>
       <c r="D49" t="s">
@@ -13285,7 +13292,7 @@
       <c r="B50" t="s">
         <v>14</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="3" t="s">
         <v>164</v>
       </c>
       <c r="D50" t="s">
@@ -13311,7 +13318,7 @@
       <c r="B51" t="s">
         <v>14</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
         <v>165</v>
       </c>
       <c r="D51" t="s">
@@ -13400,7 +13407,7 @@
       <c r="B52" t="s">
         <v>14</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
         <v>166</v>
       </c>
       <c r="D52" t="s">
@@ -13471,7 +13478,7 @@
       <c r="B53" t="s">
         <v>14</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D53" t="s">
@@ -13545,7 +13552,7 @@
       <c r="B54" t="s">
         <v>15</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="3" t="s">
         <v>168</v>
       </c>
       <c r="D54" t="s">
@@ -13574,7 +13581,7 @@
       <c r="B55" t="s">
         <v>15</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D55" t="s">
@@ -13639,7 +13646,7 @@
       <c r="B56" t="s">
         <v>15</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
         <v>170</v>
       </c>
       <c r="D56" t="s">
@@ -13716,7 +13723,7 @@
       <c r="B57" t="s">
         <v>15</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="3" t="s">
         <v>171</v>
       </c>
       <c r="D57" t="s">
@@ -13802,7 +13809,7 @@
       <c r="B58" t="s">
         <v>15</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="3" t="s">
         <v>172</v>
       </c>
       <c r="D58" t="s">
@@ -13849,7 +13856,7 @@
       <c r="B59" t="s">
         <v>15</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D59" t="s">
@@ -13884,7 +13891,7 @@
       <c r="B60" t="s">
         <v>15</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="3" t="s">
         <v>174</v>
       </c>
       <c r="D60" t="s">
@@ -13943,7 +13950,7 @@
       <c r="B61" t="s">
         <v>15</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
         <v>175</v>
       </c>
       <c r="D61" t="s">
@@ -13984,7 +13991,7 @@
       <c r="B62" t="s">
         <v>15</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>176</v>
       </c>
       <c r="D62" t="s">
@@ -14028,7 +14035,7 @@
       <c r="B63" t="s">
         <v>16</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
         <v>177</v>
       </c>
       <c r="D63" t="s">
@@ -14048,7 +14055,7 @@
       <c r="B64" t="s">
         <v>16</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
         <v>178</v>
       </c>
       <c r="D64" t="s">
@@ -14134,7 +14141,7 @@
       <c r="B65" t="s">
         <v>16</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
         <v>179</v>
       </c>
       <c r="D65" t="s">
@@ -14211,7 +14218,7 @@
       <c r="B66" t="s">
         <v>16</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D66" t="s">
@@ -14255,7 +14262,7 @@
       <c r="B67" t="s">
         <v>16</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="3" t="s">
         <v>181</v>
       </c>
       <c r="D67" t="s">
@@ -14314,7 +14321,7 @@
       <c r="B68" t="s">
         <v>16</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="3" t="s">
         <v>182</v>
       </c>
       <c r="D68" t="s">
@@ -14388,7 +14395,7 @@
       <c r="B69" t="s">
         <v>17</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="3" t="s">
         <v>183</v>
       </c>
       <c r="D69" t="s">
@@ -14423,7 +14430,7 @@
       <c r="B70" t="s">
         <v>17</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D70" t="s">
@@ -14464,7 +14471,7 @@
       <c r="B71" t="s">
         <v>17</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="3" t="s">
         <v>186</v>
       </c>
       <c r="D71" t="s">
@@ -14511,7 +14518,7 @@
       <c r="B72" t="s">
         <v>17</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="3" t="s">
         <v>187</v>
       </c>
       <c r="D72" t="s">
@@ -14591,7 +14598,7 @@
       <c r="B73" t="s">
         <v>17</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="3" t="s">
         <v>188</v>
       </c>
       <c r="D73" t="s">
@@ -14626,7 +14633,7 @@
       <c r="B74" t="s">
         <v>17</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="3" t="s">
         <v>189</v>
       </c>
       <c r="D74" t="s">
@@ -14712,7 +14719,7 @@
       <c r="B75" t="s">
         <v>17</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="3" t="s">
         <v>190</v>
       </c>
       <c r="D75" t="s">
@@ -14768,7 +14775,7 @@
       <c r="B76" t="s">
         <v>17</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="3" t="s">
         <v>191</v>
       </c>
       <c r="D76" t="s">
@@ -14806,7 +14813,7 @@
       <c r="B77" t="s">
         <v>17</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D77" t="s">
@@ -14931,7 +14938,7 @@
       <c r="B78" t="s">
         <v>17</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D78" t="s">
@@ -14981,7 +14988,7 @@
       <c r="B79" t="s">
         <v>17</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="3" t="s">
         <v>185</v>
       </c>
       <c r="D79" t="s">
@@ -15025,7 +15032,7 @@
       <c r="B80" t="s">
         <v>17</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="3" t="s">
         <v>194</v>
       </c>
       <c r="D80" t="s">
@@ -15057,7 +15064,7 @@
       <c r="B81" t="s">
         <v>17</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="3" t="s">
         <v>195</v>
       </c>
       <c r="D81" t="s">
@@ -15128,7 +15135,7 @@
       <c r="B82" t="s">
         <v>18</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D82" t="s">
@@ -15148,7 +15155,7 @@
       <c r="B83" t="s">
         <v>18</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="3" t="s">
         <v>197</v>
       </c>
       <c r="D83" t="s">
@@ -15207,7 +15214,7 @@
       <c r="B84" t="s">
         <v>18</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="3" t="s">
         <v>198</v>
       </c>
       <c r="D84" t="s">
@@ -15269,7 +15276,7 @@
       <c r="B85" t="s">
         <v>18</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="3" t="s">
         <v>199</v>
       </c>
       <c r="D85" t="s">
@@ -15397,7 +15404,7 @@
       <c r="B86" t="s">
         <v>18</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="3" t="s">
         <v>200</v>
       </c>
       <c r="D86" t="s">
@@ -15435,7 +15442,7 @@
       <c r="B87" t="s">
         <v>18</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="3" t="s">
         <v>201</v>
       </c>
       <c r="D87" t="s">
@@ -15530,7 +15537,7 @@
       <c r="B88" t="s">
         <v>18</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="3" t="s">
         <v>202</v>
       </c>
       <c r="D88" t="s">
@@ -15562,7 +15569,7 @@
       <c r="B89" t="s">
         <v>18</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D89" t="s">
@@ -15606,7 +15613,7 @@
       <c r="B90" t="s">
         <v>18</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="3" t="s">
         <v>204</v>
       </c>
       <c r="D90" t="s">
@@ -15719,7 +15726,7 @@
       <c r="B91" t="s">
         <v>3</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D91" t="s">
@@ -15778,7 +15785,7 @@
       <c r="B92" t="s">
         <v>3</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D92" t="s">
@@ -15831,7 +15838,7 @@
       <c r="B93" t="s">
         <v>3</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D93" t="s">
@@ -15896,7 +15903,7 @@
       <c r="B94" t="s">
         <v>3</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D94" t="s">
@@ -15961,7 +15968,7 @@
       <c r="B95" t="s">
         <v>3</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D95" t="s">
@@ -16008,7 +16015,7 @@
       <c r="B96" t="s">
         <v>3</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D96" t="s">
@@ -16040,7 +16047,7 @@
       <c r="B97" t="s">
         <v>3</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D97" t="s">
@@ -16078,7 +16085,7 @@
       <c r="B98" t="s">
         <v>3</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D98" t="s">
@@ -16122,7 +16129,7 @@
       <c r="B99" t="s">
         <v>3</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D99" t="s">
@@ -16181,7 +16188,7 @@
       <c r="B100" t="s">
         <v>3</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D100" t="s">
@@ -16264,7 +16271,7 @@
       <c r="B101" t="s">
         <v>3</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D101" t="s">
@@ -16293,7 +16300,7 @@
       <c r="B102" t="s">
         <v>4</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D102" t="s">
@@ -16328,7 +16335,7 @@
       <c r="B103" t="s">
         <v>4</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D103" t="s">
@@ -16378,7 +16385,7 @@
       <c r="B104" t="s">
         <v>4</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D104" t="s">
@@ -16440,7 +16447,7 @@
       <c r="B105" t="s">
         <v>4</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D105" t="s">
@@ -16541,7 +16548,7 @@
       <c r="B106" t="s">
         <v>4</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D106" t="s">
@@ -16570,7 +16577,7 @@
       <c r="B107" t="s">
         <v>4</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D107" t="s">
@@ -16635,7 +16642,7 @@
       <c r="B108" t="s">
         <v>4</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D108" t="s">
@@ -16709,7 +16716,7 @@
       <c r="B109" t="s">
         <v>4</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D109" t="s">
@@ -16756,7 +16763,7 @@
       <c r="B110" t="s">
         <v>4</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D110" t="s">
@@ -16842,7 +16849,7 @@
       <c r="B111" t="s">
         <v>4</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D111" t="s">
@@ -16907,7 +16914,7 @@
       <c r="B112" t="s">
         <v>4</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D112" t="s">
@@ -16921,7 +16928,7 @@
       <c r="B113" t="s">
         <v>5</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D113" t="s">
@@ -16971,7 +16978,7 @@
       <c r="B114" t="s">
         <v>5</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D114" t="s">
@@ -17039,7 +17046,7 @@
       <c r="B115" t="s">
         <v>5</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D115" t="s">
@@ -17095,7 +17102,7 @@
       <c r="B116" t="s">
         <v>5</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D116" t="s">
@@ -17124,7 +17131,7 @@
       <c r="B117" t="s">
         <v>5</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D117" t="s">
@@ -17174,7 +17181,7 @@
       <c r="B118" t="s">
         <v>5</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D118" t="s">
@@ -17209,7 +17216,7 @@
       <c r="B119" t="s">
         <v>5</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D119" t="s">
@@ -17235,7 +17242,7 @@
       <c r="B120" t="s">
         <v>5</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D120" t="s">
@@ -17264,7 +17271,7 @@
       <c r="B121" t="s">
         <v>5</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D121" t="s">
@@ -17347,7 +17354,7 @@
       <c r="B122" t="s">
         <v>5</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D122" t="s">
@@ -17382,7 +17389,7 @@
       <c r="B123" t="s">
         <v>5</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D123" t="s">
@@ -17408,7 +17415,7 @@
       <c r="B124" t="s">
         <v>5</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D124" t="s">
@@ -17437,7 +17444,7 @@
       <c r="B125" t="s">
         <v>6</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D125" t="s">
@@ -17484,7 +17491,7 @@
       <c r="B126" t="s">
         <v>6</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D126" t="s">
@@ -17561,7 +17568,7 @@
       <c r="B127" t="s">
         <v>6</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D127" t="s">
@@ -17674,7 +17681,7 @@
       <c r="B128" t="s">
         <v>6</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D128" t="s">
@@ -17754,7 +17761,7 @@
       <c r="B129" t="s">
         <v>6</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D129" t="s">
@@ -17813,7 +17820,7 @@
       <c r="B130" t="s">
         <v>6</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D130" t="s">
@@ -17845,7 +17852,7 @@
       <c r="B131" t="s">
         <v>7</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D131" t="s">
@@ -17874,7 +17881,7 @@
       <c r="B132" t="s">
         <v>7</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D132" t="s">
@@ -17921,7 +17928,7 @@
       <c r="B133" t="s">
         <v>7</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D133" t="s">
@@ -18019,7 +18026,7 @@
       <c r="B134" t="s">
         <v>7</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D134" t="s">
@@ -18078,7 +18085,7 @@
       <c r="B135" t="s">
         <v>7</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D135" t="s">
@@ -18122,7 +18129,7 @@
       <c r="B136" t="s">
         <v>7</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D136" t="s">
@@ -18169,7 +18176,7 @@
       <c r="B137" t="s">
         <v>7</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D137" t="s">
@@ -18201,7 +18208,7 @@
       <c r="B138" t="s">
         <v>7</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D138" t="s">
@@ -18236,7 +18243,7 @@
       <c r="B139" t="s">
         <v>7</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D139" t="s">
@@ -18259,7 +18266,7 @@
       <c r="B140" t="s">
         <v>7</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D140" t="s">
@@ -18294,7 +18301,7 @@
       <c r="B141" t="s">
         <v>7</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D141" t="s">
@@ -18335,7 +18342,7 @@
       <c r="B142" t="s">
         <v>8</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D142" t="s">
@@ -18373,7 +18380,7 @@
       <c r="B143" t="s">
         <v>8</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D143" t="s">
@@ -18495,7 +18502,7 @@
       <c r="B144" t="s">
         <v>8</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D144" t="s">
@@ -18605,7 +18612,7 @@
       <c r="B145" t="s">
         <v>8</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D145" t="s">
@@ -18682,7 +18689,7 @@
       <c r="B146" t="s">
         <v>8</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D146" t="s">
@@ -18726,7 +18733,7 @@
       <c r="B147" t="s">
         <v>8</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D147" t="s">
@@ -18845,7 +18852,7 @@
       <c r="B148" t="s">
         <v>8</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D148" t="s">
@@ -18889,7 +18896,7 @@
       <c r="B149" t="s">
         <v>8</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D149" t="s">
@@ -18924,7 +18931,7 @@
       <c r="B150" t="s">
         <v>8</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D150" t="s">
@@ -18947,7 +18954,7 @@
       <c r="B151" t="s">
         <v>8</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D151" t="s">
@@ -19009,7 +19016,7 @@
       <c r="B152" t="s">
         <v>8</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D152" t="s">
@@ -19107,7 +19114,7 @@
       <c r="B153" t="s">
         <v>8</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D153" t="s">
@@ -19151,7 +19158,7 @@
       <c r="B154" t="s">
         <v>8</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="3" t="s">
         <v>90</v>
       </c>
       <c r="D154" t="s">
@@ -19189,7 +19196,7 @@
       <c r="B155" t="s">
         <v>9</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D155" t="s">
@@ -19272,7 +19279,7 @@
       <c r="B156" t="s">
         <v>9</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D156" t="s">
@@ -19337,7 +19344,7 @@
       <c r="B157" t="s">
         <v>9</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D157" t="s">
@@ -19480,7 +19487,7 @@
       <c r="B158" t="s">
         <v>9</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D158" t="s">
@@ -19539,7 +19546,7 @@
       <c r="B159" t="s">
         <v>9</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="3" t="s">
         <v>96</v>
       </c>
       <c r="D159" t="s">
@@ -19598,7 +19605,7 @@
       <c r="B160" t="s">
         <v>9</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D160" t="s">
@@ -19627,7 +19634,7 @@
       <c r="B161" t="s">
         <v>9</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="3" t="s">
         <v>98</v>
       </c>
       <c r="D161" t="s">
@@ -19707,7 +19714,7 @@
       <c r="B162" t="s">
         <v>9</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D162" t="s">
@@ -19775,7 +19782,7 @@
       <c r="B163" t="s">
         <v>9</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="3" t="s">
         <v>100</v>
       </c>
       <c r="D163" t="s">
@@ -19807,7 +19814,7 @@
       <c r="B164" t="s">
         <v>9</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="3" t="s">
         <v>101</v>
       </c>
       <c r="D164" t="s">
@@ -19860,7 +19867,7 @@
       <c r="B165" t="s">
         <v>9</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D165" t="s">
@@ -19937,7 +19944,7 @@
       <c r="B166" t="s">
         <v>9</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D166" t="s">
@@ -19993,7 +20000,7 @@
       <c r="B167" t="s">
         <v>9</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D167" t="s">
@@ -20046,7 +20053,7 @@
       <c r="B168" t="s">
         <v>10</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D168" t="s">
@@ -20075,7 +20082,7 @@
       <c r="B169" t="s">
         <v>10</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D169" t="s">
@@ -20128,7 +20135,7 @@
       <c r="B170" t="s">
         <v>10</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D170" t="s">
@@ -20157,7 +20164,7 @@
       <c r="B171" t="s">
         <v>10</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="3" t="s">
         <v>117</v>
       </c>
       <c r="D171" t="s">
@@ -20177,7 +20184,7 @@
       <c r="B172" t="s">
         <v>10</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="3" t="s">
         <v>118</v>
       </c>
       <c r="D172" t="s">
@@ -20230,7 +20237,7 @@
       <c r="B173" t="s">
         <v>10</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="3" t="s">
         <v>119</v>
       </c>
       <c r="D173" t="s">
@@ -20277,7 +20284,7 @@
       <c r="B174" t="s">
         <v>10</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="3" t="s">
         <v>120</v>
       </c>
       <c r="D174" t="s">
@@ -20348,7 +20355,7 @@
       <c r="B175" t="s">
         <v>10</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D175" t="s">
@@ -20383,7 +20390,7 @@
       <c r="B176" t="s">
         <v>10</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D176" t="s">
@@ -20448,7 +20455,7 @@
       <c r="B177" t="s">
         <v>10</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D177" t="s">
@@ -20498,7 +20505,7 @@
       <c r="B178" t="s">
         <v>10</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="3" t="s">
         <v>106</v>
       </c>
       <c r="D178" t="s">
@@ -20620,7 +20627,7 @@
       <c r="B179" t="s">
         <v>10</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="3" t="s">
         <v>107</v>
       </c>
       <c r="D179" t="s">
@@ -20652,7 +20659,7 @@
       <c r="B180" t="s">
         <v>10</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D180" t="s">
@@ -20699,7 +20706,7 @@
       <c r="B181" t="s">
         <v>10</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="3" t="s">
         <v>109</v>
       </c>
       <c r="D181" t="s">
@@ -20731,7 +20738,7 @@
       <c r="B182" t="s">
         <v>10</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D182" t="s">
@@ -20754,7 +20761,7 @@
       <c r="B183" t="s">
         <v>10</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="3" t="s">
         <v>111</v>
       </c>
       <c r="D183" t="s">
@@ -20798,7 +20805,7 @@
       <c r="B184" t="s">
         <v>10</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D184" t="s">
@@ -20833,7 +20840,7 @@
       <c r="B185" t="s">
         <v>10</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D185" t="s">
@@ -20916,7 +20923,7 @@
       <c r="B186" t="s">
         <v>10</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D186" t="s">
@@ -20999,7 +21006,7 @@
       <c r="B187" t="s">
         <v>10</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="3" t="s">
         <v>115</v>
       </c>
       <c r="D187" t="s">

</xml_diff>